<commit_message>
Update: Part_Writter_Node file change Problem statement to Acknowledgement
</commit_message>
<xml_diff>
--- a/Documents/BaoCao/Part_Writter_Note.xlsx
+++ b/Documents/BaoCao/Part_Writter_Note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\KLTN-WeatherForecast\Documents\BaoCao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F08630-07D5-4CD4-895C-AB88B56E30A1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF86D12-4BAE-4294-B358-0F518E395B1A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{5FE9411F-E9DE-4E61-AFA8-2FF06EEE7498}"/>
   </bookViews>
@@ -36,9 +36,6 @@
     <t>Abstract</t>
   </si>
   <si>
-    <t>Problem Statement</t>
-  </si>
-  <si>
     <t>1.1 Background</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Thao</t>
+  </si>
+  <si>
+    <t>Acknowledgement</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -472,7 +472,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -489,7 +489,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -497,10 +497,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -508,7 +508,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -517,7 +517,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3"/>
     </row>
@@ -526,7 +526,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -535,7 +535,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3"/>
     </row>
@@ -544,7 +544,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -553,7 +553,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3"/>
     </row>
@@ -562,7 +562,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3"/>
     </row>

</xml_diff>

<commit_message>
Update: Part writter node that Thao will write chapter 1.1 Background and 1.2 Related work
</commit_message>
<xml_diff>
--- a/Documents/BaoCao/Part_Writter_Note.xlsx
+++ b/Documents/BaoCao/Part_Writter_Note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\KLTN-WeatherForecast\Documents\BaoCao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211E83C7-65E9-496A-9AFA-D464BF2AF95E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59341A30-EB2A-40CD-A159-9D286E76259A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -462,7 +462,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update: Update information in part writter note that Thao will write Future work part
</commit_message>
<xml_diff>
--- a/Documents/BaoCao/Part_Writter_Note.xlsx
+++ b/Documents/BaoCao/Part_Writter_Note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\KLTN-WeatherForecast\Documents\BaoCao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59341A30-EB2A-40CD-A159-9D286E76259A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C4F749-B39A-40A8-9F79-0111AE53DB35}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Part</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Hao</t>
+  </si>
+  <si>
+    <t>Future work</t>
   </si>
 </sst>
 </file>
@@ -459,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -583,6 +586,17 @@
         <v>11</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update: Add Vietnamese version of Background part in final report
</commit_message>
<xml_diff>
--- a/Documents/BaoCao/Part_Writter_Note.xlsx
+++ b/Documents/BaoCao/Part_Writter_Note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\KLTN-WeatherForecast\Documents\BaoCao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C4F749-B39A-40A8-9F79-0111AE53DB35}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCDD60B-839C-47D8-A1CA-0E969D0DAADD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -517,7 +517,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -528,7 +528,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>